<commit_message>
categorization after mela fix
</commit_message>
<xml_diff>
--- a/categorizationstudy/categorization.xlsx
+++ b/categorizationstudy/categorization.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="14">
   <si>
     <t>0+</t>
   </si>
@@ -55,6 +55,21 @@
   </si>
   <si>
     <t>ggH</t>
+  </si>
+  <si>
+    <t>0+ or a2</t>
+  </si>
+  <si>
+    <t>0+ or 0-</t>
+  </si>
+  <si>
+    <t>0+ or L1</t>
+  </si>
+  <si>
+    <t>fL1VBF=0.5</t>
+  </si>
+  <si>
+    <t>fa2VBF=-0.5</t>
   </si>
 </sst>
 </file>
@@ -419,15 +434,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -447,32 +462,32 @@
         <v>0</v>
       </c>
       <c r="B2" s="3">
-        <v>0.35391937602399998</v>
-      </c>
-      <c r="C2" s="2">
-        <v>0.85920179893100002</v>
+        <v>0.35399999999999998</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0.85899999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" s="4">
-        <v>9.1696669174699999E-2</v>
-      </c>
-      <c r="C3" s="2">
-        <v>0.85467649991500005</v>
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0.86099999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="4">
-        <v>9.2361793334899994E-2</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0.86054115014099997</v>
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0.85499999999999998</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -480,10 +495,26 @@
         <v>5</v>
       </c>
       <c r="B5" s="4">
-        <v>0.17268872842800001</v>
-      </c>
-      <c r="C5" s="2">
-        <v>0.85971561750400005</v>
+        <v>0.17199999999999999</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.222</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.23300000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -493,19 +524,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D4:D6"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>6</v>
       </c>
@@ -517,25 +548,34 @@
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="5"/>
+      <c r="B2" s="1"/>
       <c r="C2" t="s">
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
         <v>4</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
       </c>
       <c r="F2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -543,78 +583,167 @@
         <v>0</v>
       </c>
       <c r="C3" s="4">
-        <v>0.130408978354</v>
+        <v>0.502</v>
       </c>
       <c r="D3" s="4">
-        <v>4.4721384968499998E-2</v>
+        <v>0.27600000000000002</v>
       </c>
       <c r="E3" s="4">
-        <v>3.4967218113599999E-2</v>
+        <v>0.29799999999999999</v>
       </c>
       <c r="F3" s="4">
-        <v>5.7815532152100002E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="G3" s="4">
+        <v>0.53</v>
+      </c>
+      <c r="H3" s="4">
+        <v>0.53100000000000003</v>
+      </c>
+      <c r="I3" s="4">
+        <v>0.52200000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="6"/>
       <c r="B4" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="4">
-        <v>8.3339935038300006E-2</v>
+        <v>0.36499999999999999</v>
       </c>
       <c r="D4" s="4">
-        <v>0.38996258428699998</v>
+        <v>0.76400000000000001</v>
       </c>
       <c r="E4" s="4">
-        <v>0.307745057672</v>
+        <v>0.79400000000000004</v>
       </c>
       <c r="F4" s="4">
-        <v>0.33661533762500001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+        <v>0.68</v>
+      </c>
+      <c r="G4" s="4">
+        <v>0.80100000000000005</v>
+      </c>
+      <c r="H4" s="4">
+        <v>0.81699999999999995</v>
+      </c>
+      <c r="I4" s="4">
+        <v>0.71299999999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="6"/>
       <c r="B5" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="4">
-        <v>2.2082814325400001E-2</v>
+        <v>0.29499999999999998</v>
       </c>
       <c r="D5" s="4">
-        <v>0.35839105590300002</v>
+        <v>0.77600000000000002</v>
       </c>
       <c r="E5" s="4">
-        <v>0.36985584203499999</v>
+        <v>0.78200000000000003</v>
       </c>
       <c r="F5" s="4">
-        <v>0.26312819748400001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+        <v>0.67400000000000004</v>
+      </c>
+      <c r="G5" s="4">
+        <v>0.80500000000000005</v>
+      </c>
+      <c r="H5" s="4">
+        <v>0.81100000000000005</v>
+      </c>
+      <c r="I5" s="4">
+        <v>0.71799999999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="6"/>
       <c r="B6" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="4">
-        <v>4.3236402573600001E-2</v>
+        <v>0.30599999999999999</v>
       </c>
       <c r="D6" s="4">
-        <v>0.35711445877199999</v>
+        <v>0.72299999999999998</v>
       </c>
       <c r="E6" s="4">
-        <v>0.32666562019700002</v>
+        <v>0.73799999999999999</v>
       </c>
       <c r="F6" s="4">
-        <v>0.46123801307899998</v>
+        <v>0.71699999999999997</v>
+      </c>
+      <c r="G6" s="4">
+        <v>0.751</v>
+      </c>
+      <c r="H6" s="4">
+        <v>0.75900000000000001</v>
+      </c>
+      <c r="I6" s="4">
+        <v>0.73699999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="6"/>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.37</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.52900000000000003</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0.54500000000000004</v>
+      </c>
+      <c r="F7" s="4">
+        <v>0.46899999999999997</v>
+      </c>
+      <c r="G7" s="4">
+        <v>0.66300000000000003</v>
+      </c>
+      <c r="H7" s="4">
+        <v>0.66800000000000004</v>
+      </c>
+      <c r="I7" s="4">
+        <v>0.60899999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" s="6"/>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.42899999999999999</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.53500000000000003</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0.55400000000000005</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0.52700000000000002</v>
+      </c>
+      <c r="G8" s="4">
+        <v>0.66100000000000003</v>
+      </c>
+      <c r="H8" s="4">
+        <v>0.66600000000000004</v>
+      </c>
+      <c r="I8" s="4">
+        <v>0.64900000000000002</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="C1:F1"/>
-    <mergeCell ref="A3:A6"/>
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:A8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -622,19 +751,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="str">
         <f>VBF!A1&amp;" events with 2 jets"</f>
         <v>VBF events with 2 jets</v>
@@ -648,7 +777,7 @@
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="str">
         <f>VBF!A2</f>
         <v>VBF category</v>
@@ -660,18 +789,30 @@
       </c>
       <c r="D2" t="str">
         <f>VBF!D2</f>
-        <v>0-</v>
-      </c>
-      <c r="E2" t="str">
+        <v>a2</v>
+      </c>
+      <c r="E2">
         <f>VBF!E2</f>
-        <v>a2</v>
+        <v>0</v>
       </c>
       <c r="F2" t="str">
         <f>VBF!F2</f>
         <v>L1</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G2" t="str">
+        <f>VBF!G2</f>
+        <v>0+ or a2</v>
+      </c>
+      <c r="H2" t="str">
+        <f>VBF!H2</f>
+        <v>0+ or 0-</v>
+      </c>
+      <c r="I2" t="str">
+        <f>VBF!I2</f>
+        <v>0+ or L1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="str">
         <f>VBF!A3</f>
         <v>sample</v>
@@ -682,23 +823,34 @@
       </c>
       <c r="C3" s="4">
         <f>VBF!C3/(1-'not enough jets'!$B2)</f>
-        <v>0.20184629211050961</v>
+        <v>0.77708978328173373</v>
       </c>
       <c r="D3" s="4">
         <f>VBF!D3/(1-'not enough jets'!$B2)</f>
-        <v>6.9219511170731635E-2</v>
+        <v>0.4272445820433437</v>
       </c>
       <c r="E3" s="4">
         <f>VBF!E3/(1-'not enough jets'!$B2)</f>
-        <v>5.4122065909376245E-2</v>
+        <v>0.46130030959752316</v>
       </c>
       <c r="F3" s="4">
         <f>VBF!F3/(1-'not enough jets'!$B2)</f>
-        <v>8.9486559427059492E-2</v>
-      </c>
-      <c r="H3" s="4"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.41021671826625389</v>
+      </c>
+      <c r="G3" s="4">
+        <f>VBF!G3/(1-'not enough jets'!$B2)</f>
+        <v>0.82043343653250778</v>
+      </c>
+      <c r="H3" s="4">
+        <f>VBF!H3/(1-'not enough jets'!$B2)</f>
+        <v>0.82198142414860687</v>
+      </c>
+      <c r="I3" s="4">
+        <f>VBF!I3/(1-'not enough jets'!$B2)</f>
+        <v>0.80804953560371517</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="6"/>
       <c r="B4" t="str">
         <f>VBF!B4</f>
@@ -706,22 +858,34 @@
       </c>
       <c r="C4" s="4">
         <f>VBF!C4/(1-'not enough jets'!$B3)</f>
-        <v>9.1753417839584392E-2</v>
+        <v>0.40198237885462551</v>
       </c>
       <c r="D4" s="4">
         <f>VBF!D4/(1-'not enough jets'!$B3)</f>
-        <v>0.42933078747236703</v>
+        <v>0.84140969162995594</v>
       </c>
       <c r="E4" s="4">
         <f>VBF!E4/(1-'not enough jets'!$B3)</f>
-        <v>0.33881308944708766</v>
+        <v>0.87444933920704848</v>
       </c>
       <c r="F4" s="4">
         <f>VBF!F4/(1-'not enough jets'!$B3)</f>
-        <v>0.370597933753194</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.74889867841409696</v>
+      </c>
+      <c r="G4" s="4">
+        <f>VBF!G4/(1-'not enough jets'!$B3)</f>
+        <v>0.88215859030837007</v>
+      </c>
+      <c r="H4" s="4">
+        <f>VBF!H4/(1-'not enough jets'!$B3)</f>
+        <v>0.89977973568281933</v>
+      </c>
+      <c r="I4" s="4">
+        <f>VBF!I4/(1-'not enough jets'!$B3)</f>
+        <v>0.78524229074889862</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="6"/>
       <c r="B5" t="str">
         <f>VBF!B5</f>
@@ -729,22 +893,34 @@
       </c>
       <c r="C5" s="4">
         <f>VBF!C5/(1-'not enough jets'!$B4)</f>
-        <v>2.4329974392041112E-2</v>
+        <v>0.32488986784140966</v>
       </c>
       <c r="D5" s="4">
         <f>VBF!D5/(1-'not enough jets'!$B4)</f>
-        <v>0.39486113880091323</v>
+        <v>0.85462555066079293</v>
       </c>
       <c r="E5" s="4">
         <f>VBF!E5/(1-'not enough jets'!$B4)</f>
-        <v>0.40749258825710638</v>
+        <v>0.86123348017621149</v>
       </c>
       <c r="F5" s="4">
         <f>VBF!F5/(1-'not enough jets'!$B4)</f>
-        <v>0.28990427634244464</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.74229074889867841</v>
+      </c>
+      <c r="G5" s="4">
+        <f>VBF!G5/(1-'not enough jets'!$B4)</f>
+        <v>0.88656387665198244</v>
+      </c>
+      <c r="H5" s="4">
+        <f>VBF!H5/(1-'not enough jets'!$B4)</f>
+        <v>0.89317180616740088</v>
+      </c>
+      <c r="I5" s="4">
+        <f>VBF!I5/(1-'not enough jets'!$B4)</f>
+        <v>0.79074889867841403</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="6"/>
       <c r="B6" t="str">
         <f>VBF!B6</f>
@@ -752,19 +928,101 @@
       </c>
       <c r="C6" s="4">
         <f>VBF!C6/(1-'not enough jets'!$B5)</f>
-        <v>5.2261348369453689E-2</v>
+        <v>0.36956521739130432</v>
       </c>
       <c r="D6" s="4">
         <f>VBF!D6/(1-'not enough jets'!$B5)</f>
-        <v>0.43165670654218896</v>
+        <v>0.87318840579710133</v>
       </c>
       <c r="E6" s="4">
         <f>VBF!E6/(1-'not enough jets'!$B5)</f>
-        <v>0.39485213295389104</v>
+        <v>0.89130434782608692</v>
       </c>
       <c r="F6" s="4">
         <f>VBF!F6/(1-'not enough jets'!$B5)</f>
-        <v>0.55751447964994749</v>
+        <v>0.8659420289855071</v>
+      </c>
+      <c r="G6" s="4">
+        <f>VBF!G6/(1-'not enough jets'!$B5)</f>
+        <v>0.90700483091787432</v>
+      </c>
+      <c r="H6" s="4">
+        <f>VBF!H6/(1-'not enough jets'!$B5)</f>
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="I6" s="4">
+        <f>VBF!I6/(1-'not enough jets'!$B5)</f>
+        <v>0.89009661835748788</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="6"/>
+      <c r="B7" t="str">
+        <f>VBF!B7</f>
+        <v>fa2VBF=-0.5</v>
+      </c>
+      <c r="C7" s="4">
+        <f>VBF!C7/(1-'not enough jets'!$B6)</f>
+        <v>0.47557840616966579</v>
+      </c>
+      <c r="D7" s="4">
+        <f>VBF!D7/(1-'not enough jets'!$B6)</f>
+        <v>0.67994858611825193</v>
+      </c>
+      <c r="E7" s="4">
+        <f>VBF!E7/(1-'not enough jets'!$B6)</f>
+        <v>0.7005141388174807</v>
+      </c>
+      <c r="F7" s="4">
+        <f>VBF!F7/(1-'not enough jets'!$B6)</f>
+        <v>0.60282776349614386</v>
+      </c>
+      <c r="G7" s="4">
+        <f>VBF!G7/(1-'not enough jets'!$B6)</f>
+        <v>0.8521850899742931</v>
+      </c>
+      <c r="H7" s="4">
+        <f>VBF!H7/(1-'not enough jets'!$B6)</f>
+        <v>0.8586118251928021</v>
+      </c>
+      <c r="I7" s="4">
+        <f>VBF!I7/(1-'not enough jets'!$B6)</f>
+        <v>0.78277634961439579</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" s="6"/>
+      <c r="B8" t="str">
+        <f>VBF!B8</f>
+        <v>fL1VBF=0.5</v>
+      </c>
+      <c r="C8" s="4">
+        <f>VBF!C8/(1-'not enough jets'!$B7)</f>
+        <v>0.55932203389830504</v>
+      </c>
+      <c r="D8" s="4">
+        <f>VBF!D8/(1-'not enough jets'!$B7)</f>
+        <v>0.69752281616688394</v>
+      </c>
+      <c r="E8" s="4">
+        <f>VBF!E8/(1-'not enough jets'!$B7)</f>
+        <v>0.72229465449804442</v>
+      </c>
+      <c r="F8" s="4">
+        <f>VBF!F8/(1-'not enough jets'!$B7)</f>
+        <v>0.68709256844850064</v>
+      </c>
+      <c r="G8" s="4">
+        <f>VBF!G8/(1-'not enough jets'!$B7)</f>
+        <v>0.8617992177314211</v>
+      </c>
+      <c r="H8" s="4">
+        <f>VBF!H8/(1-'not enough jets'!$B7)</f>
+        <v>0.86831812255541074</v>
+      </c>
+      <c r="I8" s="4">
+        <f>VBF!I8/(1-'not enough jets'!$B7)</f>
+        <v>0.84615384615384615</v>
       </c>
     </row>
   </sheetData>
@@ -772,7 +1030,7 @@
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="A3:A8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -780,19 +1038,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>8</v>
       </c>
@@ -804,7 +1062,7 @@
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>7</v>
       </c>
@@ -813,16 +1071,25 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
         <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
       </c>
       <c r="F2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -830,70 +1097,106 @@
         <v>0</v>
       </c>
       <c r="C3" s="4">
-        <v>5.7852088415800001E-3</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="D3" s="4">
-        <v>2.7356094274100001E-3</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="E3" s="4">
-        <v>1.5365792753599999E-3</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="F3" s="4">
-        <v>2.7398972748800001E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+        <v>1.9E-2</v>
+      </c>
+      <c r="G3" s="4">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="H3" s="4">
+        <v>5.5E-2</v>
+      </c>
+      <c r="I3" s="4">
+        <v>4.3999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="6"/>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4" s="4">
-        <v>5.4744015290799997E-3</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="D4" s="4">
-        <v>2.7837707509699998E-3</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="E4" s="4">
-        <v>1.5803676684799999E-3</v>
+        <v>0.03</v>
       </c>
       <c r="F4" s="4">
-        <v>2.8542188618199999E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="G4" s="4">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="H4" s="4">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="I4" s="4">
+        <v>4.2999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="6"/>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" s="4">
-        <v>5.2700447595E-3</v>
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="D5" s="4">
-        <v>2.6779122635000002E-3</v>
+        <v>2.8000000000000001E-2</v>
       </c>
       <c r="E5" s="4">
-        <v>1.6523558931099999E-3</v>
+        <v>3.3000000000000002E-2</v>
       </c>
       <c r="F5" s="4">
-        <v>2.7181608305500001E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+        <v>1.9E-2</v>
+      </c>
+      <c r="G5" s="4">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="H5" s="4">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="I5" s="4">
+        <v>4.4999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="6"/>
       <c r="B6" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="4">
-        <v>5.6405999117800001E-3</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="D6" s="4">
-        <v>2.6090743411000001E-3</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="E6" s="4">
-        <v>1.68420082913E-3</v>
+        <v>3.1E-2</v>
       </c>
       <c r="F6" s="4">
-        <v>2.70698926559E-3</v>
+        <v>1.9E-2</v>
+      </c>
+      <c r="G6" s="4">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="H6" s="4">
+        <v>5.5E-2</v>
+      </c>
+      <c r="I6" s="4">
+        <v>4.3999999999999997E-2</v>
       </c>
     </row>
   </sheetData>
@@ -909,19 +1212,19 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="str">
         <f>ggH!A1&amp;" events with 2 jets"</f>
         <v>ggH events with 2 jets</v>
@@ -935,7 +1238,7 @@
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="str">
         <f>ggH!A2</f>
         <v>VBF category</v>
@@ -947,18 +1250,30 @@
       </c>
       <c r="D2" t="str">
         <f>ggH!D2</f>
-        <v>0-</v>
+        <v>a2</v>
       </c>
       <c r="E2" t="str">
         <f>ggH!E2</f>
-        <v>a2</v>
+        <v>0-</v>
       </c>
       <c r="F2" t="str">
         <f>ggH!F2</f>
         <v>L1</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G2" t="str">
+        <f>ggH!G2</f>
+        <v>0+ or a2</v>
+      </c>
+      <c r="H2" t="str">
+        <f>ggH!H2</f>
+        <v>0+ or 0-</v>
+      </c>
+      <c r="I2" t="str">
+        <f>ggH!I2</f>
+        <v>0+ or L1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="str">
         <f>ggH!A3</f>
         <v>sample</v>
@@ -969,69 +1284,104 @@
       </c>
       <c r="C3" s="4">
         <f>ggH!C3/(1-'not enough jets'!$C2)</f>
-        <v>4.1088655946285017E-2</v>
+        <v>0.25531914893617019</v>
       </c>
       <c r="D3" s="4">
         <f>ggH!D3/(1-'not enough jets'!$C2)</f>
-        <v>1.9429292467091814E-2</v>
+        <v>0.18439716312056734</v>
       </c>
       <c r="E3" s="4">
         <f>ggH!E3/(1-'not enough jets'!$C2)</f>
-        <v>1.0913344515012514E-2</v>
+        <v>0.22695035460992907</v>
       </c>
       <c r="F3" s="4">
         <f>ggH!F3/(1-'not enough jets'!$C2)</f>
-        <v>1.9459746318330289E-2</v>
-      </c>
-      <c r="H3" s="4"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.13475177304964536</v>
+      </c>
+      <c r="G3" s="4">
+        <f>ggH!G3/(1-'not enough jets'!$C2)</f>
+        <v>0.36879432624113467</v>
+      </c>
+      <c r="H3" s="4">
+        <f>ggH!H3/(1-'not enough jets'!$C2)</f>
+        <v>0.39007092198581556</v>
+      </c>
+      <c r="I3" s="4">
+        <f>ggH!I3/(1-'not enough jets'!$C2)</f>
+        <v>0.31205673758865243</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="6"/>
       <c r="B4" t="str">
         <f>ggH!B4</f>
-        <v>0-</v>
+        <v>a2</v>
       </c>
       <c r="C4" s="4">
         <f>ggH!C4/(1-'not enough jets'!$C3)</f>
-        <v>3.7670449210747151E-2</v>
+        <v>0.25899280575539563</v>
       </c>
       <c r="D4" s="4">
         <f>ggH!D4/(1-'not enough jets'!$C3)</f>
-        <v>1.9155681973953061E-2</v>
+        <v>0.18705035971223019</v>
       </c>
       <c r="E4" s="4">
         <f>ggH!E4/(1-'not enough jets'!$C3)</f>
-        <v>1.087482525232079E-2</v>
+        <v>0.21582733812949637</v>
       </c>
       <c r="F4" s="4">
         <f>ggH!F4/(1-'not enough jets'!$C3)</f>
-        <v>1.9640449480989398E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.12949640287769781</v>
+      </c>
+      <c r="G4" s="4">
+        <f>ggH!G4/(1-'not enough jets'!$C3)</f>
+        <v>0.36690647482014382</v>
+      </c>
+      <c r="H4" s="4">
+        <f>ggH!H4/(1-'not enough jets'!$C3)</f>
+        <v>0.3884892086330935</v>
+      </c>
+      <c r="I4" s="4">
+        <f>ggH!I4/(1-'not enough jets'!$C3)</f>
+        <v>0.30935251798561147</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="6"/>
       <c r="B5" t="str">
         <f>ggH!B5</f>
-        <v>a2</v>
+        <v>0-</v>
       </c>
       <c r="C5" s="4">
         <f>ggH!C5/(1-'not enough jets'!$C4)</f>
-        <v>3.77892458228953E-2</v>
+        <v>0.2551724137931034</v>
       </c>
       <c r="D5" s="4">
         <f>ggH!D5/(1-'not enough jets'!$C4)</f>
-        <v>1.9202167995846123E-2</v>
+        <v>0.19310344827586204</v>
       </c>
       <c r="E5" s="4">
         <f>ggH!E5/(1-'not enough jets'!$C4)</f>
-        <v>1.1848340171890242E-2</v>
+        <v>0.22758620689655171</v>
       </c>
       <c r="F5" s="4">
         <f>ggH!F5/(1-'not enough jets'!$C4)</f>
-        <v>1.9490773323444146E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.13103448275862067</v>
+      </c>
+      <c r="G5" s="4">
+        <f>ggH!G5/(1-'not enough jets'!$C4)</f>
+        <v>0.37241379310344824</v>
+      </c>
+      <c r="H5" s="4">
+        <f>ggH!H5/(1-'not enough jets'!$C4)</f>
+        <v>0.39310344827586202</v>
+      </c>
+      <c r="I5" s="4">
+        <f>ggH!I5/(1-'not enough jets'!$C4)</f>
+        <v>0.31034482758620685</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="6"/>
       <c r="B6" t="str">
         <f>ggH!B6</f>
@@ -1039,19 +1389,31 @@
       </c>
       <c r="C6" s="4">
         <f>ggH!C6/(1-'not enough jets'!$C5)</f>
-        <v>4.0208324058744284E-2</v>
+        <v>0.25714285714285712</v>
       </c>
       <c r="D6" s="4">
         <f>ggH!D6/(1-'not enough jets'!$C5)</f>
-        <v>1.8598466163362089E-2</v>
+        <v>0.18571428571428569</v>
       </c>
       <c r="E6" s="4">
         <f>ggH!E6/(1-'not enough jets'!$C5)</f>
-        <v>1.2005618866220001E-2</v>
+        <v>0.22142857142857142</v>
       </c>
       <c r="F6" s="4">
         <f>ggH!F6/(1-'not enough jets'!$C5)</f>
-        <v>1.9296440683033173E-2</v>
+        <v>0.1357142857142857</v>
+      </c>
+      <c r="G6" s="4">
+        <f>ggH!G6/(1-'not enough jets'!$C5)</f>
+        <v>0.37142857142857139</v>
+      </c>
+      <c r="H6" s="4">
+        <f>ggH!H6/(1-'not enough jets'!$C5)</f>
+        <v>0.39285714285714285</v>
+      </c>
+      <c r="I6" s="4">
+        <f>ggH!I6/(1-'not enough jets'!$C5)</f>
+        <v>0.31428571428571422</v>
       </c>
     </row>
   </sheetData>

</xml_diff>